<commit_message>
D3_components_flare_TD_E_GRAVES_AESI codebook completed for general flares - component strategy not supported yet
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_components_flare_TD_E_GRAVES_AESI.xlsx
+++ b/i_codebooks/D3_components_flare_TD_E_GRAVES_AESI.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="201">
   <si>
     <t>metadata_content</t>
   </si>
@@ -176,9 +176,6 @@
     <t>most recent date when a record of DP_ANTITHYROID has started either for the first time or after a gap of 90 days</t>
   </si>
   <si>
-    <t>use codelist DP_ANTITHYROID, merge all peiods of 90 days after each record, this binary is 1 for such periods and 0 for the other periods</t>
-  </si>
-  <si>
     <t>use the corresponding conceptsetdataset  and keep track of most recent date</t>
   </si>
   <si>
@@ -572,10 +569,67 @@
     <t>max(last_O_FLARE_AESI,start_DP_ANTITHYROID,last_E_THYROIDSTORM_AESI,last_TP_THYROIDECTOMY_AESI,last_TP_RADIOIODINEABLA_AESI,last_EMG_GD,last_HOSP_GD)</t>
   </si>
   <si>
-    <t>TD dataset that contains all the variables needed to identify a flare of {ImmDis}, as per Table 4 of the protocol and codelist names in the BRIDGE metadata table</t>
-  </si>
-  <si>
     <t>person in the E_GRAVES_AESI cohort</t>
+  </si>
+  <si>
+    <t>DP_ANTITHYROID</t>
+  </si>
+  <si>
+    <t>medicinal_product_id</t>
+  </si>
+  <si>
+    <t>medicinal_product_atc_code</t>
+  </si>
+  <si>
+    <t>date_prescription</t>
+  </si>
+  <si>
+    <t>disp_number_medicinal_product</t>
+  </si>
+  <si>
+    <t>presc_quantity_per_day</t>
+  </si>
+  <si>
+    <t>presc_quantity_unit</t>
+  </si>
+  <si>
+    <t>presc_duration_days</t>
+  </si>
+  <si>
+    <t>product_lot_number</t>
+  </si>
+  <si>
+    <t>indication_code</t>
+  </si>
+  <si>
+    <t>indication_code_vocabulary</t>
+  </si>
+  <si>
+    <t>origin_of_drug_record</t>
+  </si>
+  <si>
+    <t>prescriber_speciality</t>
+  </si>
+  <si>
+    <t>prescriber_speciality_vocabulary</t>
+  </si>
+  <si>
+    <t>meaing_renamed</t>
+  </si>
+  <si>
+    <t>TD dataset that contains all the variables needed to identify a flare of {ImmDis}, as per Table 4 of the protocol and codelist names in the BRIDGE metadata table, presneted as tome-dependent variables, starting from the date of entry in the cohort</t>
+  </si>
+  <si>
+    <t>use codelist DP_ANTITHYROID, merge all peiods of 90 days after each record, this binary is 1 for such periods after the first day, and 0 for the other periods including the first day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use codelist DP_ANTITHYROID, merge all periods of 90 days after each record, and keep the most recent start date such a period until a new such period starts </t>
+  </si>
+  <si>
+    <t>use the corresponding conceptsetdataset  and keep track of most recent date happened when bool_DP_ANTITHYROID_90_days == 0</t>
+  </si>
+  <si>
+    <t>P03</t>
   </si>
 </sst>
 </file>
@@ -647,7 +701,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -672,8 +726,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -696,11 +756,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -758,22 +831,32 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1057,7 +1140,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,15 +1162,15 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1095,7 +1178,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1103,7 +1186,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1111,7 +1194,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1154,10 +1237,10 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1222,7 +1305,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>34</v>
@@ -1233,7 +1316,7 @@
         <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1269,36 +1352,36 @@
         <v>42</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>43</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>41</v>
       </c>
@@ -1309,13 +1392,13 @@
         <v>44</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>50</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -1329,261 +1412,261 @@
         <v>42</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>42</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>50</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>156</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>157</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>42</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>79</v>
-      </c>
       <c r="G15" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K15" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>43</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>49</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>44</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>86</v>
-      </c>
       <c r="G18" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>88</v>
-      </c>
       <c r="G19" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>90</v>
-      </c>
       <c r="G20" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>42</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>42</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>42</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1630,10 +1713,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>57</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1642,77 +1725,77 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
         <v>91</v>
       </c>
-      <c r="B5" t="s">
-        <v>92</v>
-      </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -1744,10 +1827,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AM50"/>
+  <dimension ref="A2:AM61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1774,595 +1857,1771 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="N2" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="T2" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="V2" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="W2" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y2" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z2" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA2" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB2" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC2" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD2" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE2" s="32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="33">
+        <v>100</v>
+      </c>
+      <c r="C3" s="33">
+        <v>190</v>
+      </c>
+      <c r="D3" s="33">
+        <v>2190</v>
+      </c>
+      <c r="E3" s="33">
+        <v>100</v>
+      </c>
+      <c r="F3" s="33">
+        <v>199</v>
+      </c>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="33"/>
+      <c r="Y3" s="33"/>
+      <c r="Z3" s="33"/>
+      <c r="AA3" s="33"/>
+      <c r="AB3" s="33"/>
+      <c r="AC3" s="33"/>
+      <c r="AD3" s="33"/>
+      <c r="AE3" s="33"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="33">
+        <v>100</v>
+      </c>
+      <c r="C4" s="33">
+        <v>190</v>
+      </c>
+      <c r="D4" s="33">
+        <v>2190</v>
+      </c>
+      <c r="E4" s="33">
+        <v>200</v>
+      </c>
+      <c r="F4" s="33">
+        <v>2190</v>
+      </c>
+      <c r="G4" s="33">
+        <v>200</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33">
+        <v>200</v>
+      </c>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="33"/>
+      <c r="AA4" s="33"/>
+      <c r="AB4" s="33"/>
+      <c r="AC4" s="33"/>
+      <c r="AD4" s="33"/>
+      <c r="AE4" s="33">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="32">
+        <v>200</v>
+      </c>
+      <c r="C5" s="32">
+        <v>290</v>
+      </c>
+      <c r="D5" s="32">
+        <v>2190</v>
+      </c>
+      <c r="E5" s="32">
+        <v>200</v>
+      </c>
+      <c r="F5" s="32">
+        <v>299</v>
+      </c>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32">
+        <v>0</v>
+      </c>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="32"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
+      <c r="AA5" s="32"/>
+      <c r="AB5" s="32"/>
+      <c r="AC5" s="32"/>
+      <c r="AD5" s="32"/>
+      <c r="AE5" s="32"/>
+    </row>
+    <row r="6" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="32">
+        <v>200</v>
+      </c>
+      <c r="C6" s="32">
+        <v>290</v>
+      </c>
+      <c r="D6" s="32">
+        <v>2190</v>
+      </c>
+      <c r="E6" s="32">
+        <v>300</v>
+      </c>
+      <c r="F6" s="32">
+        <v>300</v>
+      </c>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32">
+        <v>0</v>
+      </c>
+      <c r="I6" s="32">
+        <v>300</v>
+      </c>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="32"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="32"/>
+      <c r="AA6" s="32"/>
+      <c r="AB6" s="32"/>
+      <c r="AC6" s="32"/>
+      <c r="AD6" s="32"/>
+      <c r="AE6" s="32">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="32">
+        <v>200</v>
+      </c>
+      <c r="C7" s="32">
+        <v>290</v>
+      </c>
+      <c r="D7" s="32">
+        <v>2190</v>
+      </c>
+      <c r="E7" s="32">
+        <v>301</v>
+      </c>
+      <c r="F7" s="32">
+        <v>460</v>
+      </c>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32">
+        <v>1</v>
+      </c>
+      <c r="I7" s="32">
+        <v>300</v>
+      </c>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="32"/>
+      <c r="AA7" s="32"/>
+      <c r="AB7" s="32"/>
+      <c r="AC7" s="32"/>
+      <c r="AD7" s="32"/>
+      <c r="AE7" s="32">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="32">
+        <v>200</v>
+      </c>
+      <c r="C8" s="32">
+        <v>290</v>
+      </c>
+      <c r="D8" s="32">
+        <v>2190</v>
+      </c>
+      <c r="E8" s="32">
+        <v>461</v>
+      </c>
+      <c r="F8" s="32">
+        <v>499</v>
+      </c>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32">
+        <v>0</v>
+      </c>
+      <c r="I8" s="32">
+        <v>300</v>
+      </c>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="32"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="32"/>
+      <c r="Z8" s="32"/>
+      <c r="AA8" s="32"/>
+      <c r="AB8" s="32"/>
+      <c r="AC8" s="32"/>
+      <c r="AD8" s="32"/>
+      <c r="AE8" s="32">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="32">
+        <v>200</v>
+      </c>
+      <c r="C9" s="32">
+        <v>290</v>
+      </c>
+      <c r="D9" s="32">
+        <v>2190</v>
+      </c>
+      <c r="E9" s="32">
+        <v>500</v>
+      </c>
+      <c r="F9" s="32">
+        <v>500</v>
+      </c>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32">
+        <v>0</v>
+      </c>
+      <c r="I9" s="32">
+        <v>500</v>
+      </c>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="32"/>
+      <c r="AA9" s="32"/>
+      <c r="AB9" s="32"/>
+      <c r="AC9" s="32"/>
+      <c r="AD9" s="32"/>
+      <c r="AE9" s="32">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="32">
+        <v>200</v>
+      </c>
+      <c r="C10" s="32">
+        <v>290</v>
+      </c>
+      <c r="D10" s="32">
+        <v>2190</v>
+      </c>
+      <c r="E10" s="32">
+        <v>501</v>
+      </c>
+      <c r="F10" s="32">
+        <v>590</v>
+      </c>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32">
+        <v>1</v>
+      </c>
+      <c r="I10" s="32">
+        <v>500</v>
+      </c>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="32"/>
+      <c r="AA10" s="32"/>
+      <c r="AB10" s="32"/>
+      <c r="AC10" s="32"/>
+      <c r="AD10" s="32"/>
+      <c r="AE10" s="32">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="32">
+        <v>200</v>
+      </c>
+      <c r="C11" s="32">
+        <v>290</v>
+      </c>
+      <c r="D11" s="32">
+        <v>2190</v>
+      </c>
+      <c r="E11" s="32">
+        <v>591</v>
+      </c>
+      <c r="F11" s="32">
+        <v>599</v>
+      </c>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32">
+        <v>0</v>
+      </c>
+      <c r="I11" s="32">
+        <v>500</v>
+      </c>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="32"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="32"/>
+      <c r="Z11" s="32"/>
+      <c r="AA11" s="32"/>
+      <c r="AB11" s="32"/>
+      <c r="AC11" s="32"/>
+      <c r="AD11" s="32"/>
+      <c r="AE11" s="32">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="32">
+        <v>200</v>
+      </c>
+      <c r="C12" s="32">
+        <v>290</v>
+      </c>
+      <c r="D12" s="32">
+        <v>2190</v>
+      </c>
+      <c r="E12" s="32">
+        <v>600</v>
+      </c>
+      <c r="F12" s="32">
+        <v>2190</v>
+      </c>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32">
+        <v>0</v>
+      </c>
+      <c r="I12" s="32">
+        <v>500</v>
+      </c>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32">
+        <v>600</v>
+      </c>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="32"/>
+      <c r="AA12" s="32"/>
+      <c r="AB12" s="32"/>
+      <c r="AC12" s="32"/>
+      <c r="AD12" s="32"/>
+      <c r="AE12" s="32">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" s="33">
+        <v>100</v>
+      </c>
+      <c r="C13" s="33">
+        <v>190</v>
+      </c>
+      <c r="D13" s="33">
+        <v>2190</v>
+      </c>
+      <c r="E13" s="33">
+        <v>100</v>
+      </c>
+      <c r="F13" s="33">
+        <v>499</v>
+      </c>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="33"/>
+      <c r="U13" s="33"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="33"/>
+      <c r="Y13" s="33"/>
+      <c r="Z13" s="33"/>
+      <c r="AA13" s="33"/>
+      <c r="AB13" s="33"/>
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="33"/>
+      <c r="AE13" s="33"/>
+    </row>
+    <row r="14" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" s="33">
+        <v>100</v>
+      </c>
+      <c r="C14" s="33">
+        <v>190</v>
+      </c>
+      <c r="D14" s="33">
+        <v>2190</v>
+      </c>
+      <c r="E14" s="33">
+        <v>500</v>
+      </c>
+      <c r="F14" s="33">
+        <v>500</v>
+      </c>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>500</v>
+      </c>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="33"/>
+      <c r="U14" s="33"/>
+      <c r="V14" s="33"/>
+      <c r="W14" s="33"/>
+      <c r="X14" s="33"/>
+      <c r="Y14" s="33"/>
+      <c r="Z14" s="33"/>
+      <c r="AA14" s="33"/>
+      <c r="AB14" s="33"/>
+      <c r="AC14" s="33"/>
+      <c r="AD14" s="33"/>
+      <c r="AE14" s="33">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="33">
+        <v>100</v>
+      </c>
+      <c r="C15" s="33">
+        <v>190</v>
+      </c>
+      <c r="D15" s="33">
+        <v>2190</v>
+      </c>
+      <c r="E15" s="33">
+        <v>501</v>
+      </c>
+      <c r="F15" s="33">
+        <v>549</v>
+      </c>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33">
+        <v>1</v>
+      </c>
+      <c r="I15" s="33">
+        <v>500</v>
+      </c>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="33"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="33"/>
+      <c r="Z15" s="33"/>
+      <c r="AA15" s="33"/>
+      <c r="AB15" s="33"/>
+      <c r="AC15" s="33"/>
+      <c r="AD15" s="33"/>
+      <c r="AE15" s="33">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" s="33">
+        <v>100</v>
+      </c>
+      <c r="C16" s="33">
+        <v>190</v>
+      </c>
+      <c r="D16" s="33">
+        <v>2190</v>
+      </c>
+      <c r="E16" s="33">
+        <v>550</v>
+      </c>
+      <c r="F16" s="33">
+        <v>590</v>
+      </c>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33">
+        <v>1</v>
+      </c>
+      <c r="I16" s="33">
+        <v>500</v>
+      </c>
+      <c r="J16" s="33">
+        <v>550</v>
+      </c>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="33"/>
+      <c r="U16" s="33"/>
+      <c r="V16" s="33"/>
+      <c r="W16" s="33"/>
+      <c r="X16" s="33"/>
+      <c r="Y16" s="33"/>
+      <c r="Z16" s="33"/>
+      <c r="AA16" s="33"/>
+      <c r="AB16" s="33"/>
+      <c r="AC16" s="33"/>
+      <c r="AD16" s="33"/>
+      <c r="AE16" s="33">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="33">
+        <v>100</v>
+      </c>
+      <c r="C17" s="33">
+        <v>190</v>
+      </c>
+      <c r="D17" s="33">
+        <v>2190</v>
+      </c>
+      <c r="E17" s="33">
+        <v>591</v>
+      </c>
+      <c r="F17" s="33">
+        <v>699</v>
+      </c>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <v>500</v>
+      </c>
+      <c r="J17" s="33">
+        <v>550</v>
+      </c>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="33"/>
+      <c r="T17" s="33"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="33"/>
+      <c r="X17" s="33"/>
+      <c r="Y17" s="33"/>
+      <c r="Z17" s="33"/>
+      <c r="AA17" s="33"/>
+      <c r="AB17" s="33"/>
+      <c r="AC17" s="33"/>
+      <c r="AD17" s="33"/>
+      <c r="AE17" s="33">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" s="33">
+        <v>100</v>
+      </c>
+      <c r="C18" s="33">
+        <v>190</v>
+      </c>
+      <c r="D18" s="33">
+        <v>2190</v>
+      </c>
+      <c r="E18" s="33">
+        <v>700</v>
+      </c>
+      <c r="F18" s="33">
+        <v>2190</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33">
+        <v>500</v>
+      </c>
+      <c r="J18" s="33">
+        <v>550</v>
+      </c>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="33">
+        <v>700</v>
+      </c>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="33"/>
+      <c r="Y18" s="33"/>
+      <c r="Z18" s="33"/>
+      <c r="AA18" s="33"/>
+      <c r="AB18" s="33"/>
+      <c r="AC18" s="33"/>
+      <c r="AD18" s="33"/>
+      <c r="AE18" s="33">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="M23" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="N2" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="P2" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="R2" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="T2" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="U2" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="V2" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="W2" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="X2" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y2" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z2" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA2" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB2" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC2" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="AD2" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="AE2" s="32" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>99</v>
-      </c>
-      <c r="M3" s="14"/>
-    </row>
-    <row r="6" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="L9" s="11"/>
-    </row>
-    <row r="17" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:39" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+      <c r="N23" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="O23" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="P23" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q23" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="R23" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="S23" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="T23" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="U23" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="V23" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W23" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="X23" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y23" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z23" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA23" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB23" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC23" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD23" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE23" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="AF23" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG23" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AH23" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="AI23" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ23" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK23" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="AL23" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="AM23" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A24" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35">
+        <v>2190</v>
+      </c>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35">
+        <v>1</v>
+      </c>
+      <c r="H24" s="35">
+        <v>100</v>
+      </c>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35">
+        <v>1</v>
+      </c>
+      <c r="L24" s="35">
+        <v>190</v>
+      </c>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="20">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="20">
+        <v>150</v>
+      </c>
+      <c r="R24" s="20"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="20">
+        <v>1</v>
+      </c>
+      <c r="U24" s="20">
+        <v>240</v>
+      </c>
+      <c r="V24" s="20"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="20">
+        <v>100</v>
+      </c>
+      <c r="AA24" s="20"/>
+      <c r="AB24" s="20"/>
+      <c r="AC24" s="20">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="20">
+        <v>190</v>
+      </c>
+      <c r="AE24" s="35"/>
+      <c r="AF24" s="35"/>
+      <c r="AG24" s="35"/>
+      <c r="AH24" s="35"/>
+      <c r="AI24" s="35"/>
+      <c r="AJ24" s="35"/>
+      <c r="AK24" s="35"/>
+      <c r="AL24" s="35"/>
+      <c r="AM24" s="35"/>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A25" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23">
+        <v>2190</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23">
+        <v>1</v>
+      </c>
+      <c r="H25" s="23">
+        <v>200</v>
+      </c>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23">
+        <v>1</v>
+      </c>
+      <c r="L25" s="23">
+        <v>290</v>
+      </c>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
+      <c r="U25" s="23"/>
+      <c r="V25" s="23"/>
+      <c r="W25" s="23"/>
+      <c r="X25" s="23"/>
+      <c r="Y25" s="23"/>
+      <c r="Z25" s="23"/>
+      <c r="AA25" s="23"/>
+      <c r="AB25" s="23"/>
+      <c r="AC25" s="23"/>
+      <c r="AD25" s="23"/>
+      <c r="AE25" s="23"/>
+      <c r="AF25" s="23"/>
+      <c r="AG25" s="23"/>
+      <c r="AH25" s="23"/>
+      <c r="AI25" s="23"/>
+      <c r="AJ25" s="23"/>
+      <c r="AK25" s="23"/>
+      <c r="AL25" s="23"/>
+      <c r="AM25" s="23"/>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A26" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35">
+        <v>2190</v>
+      </c>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35">
+        <v>1</v>
+      </c>
+      <c r="H26" s="35">
+        <v>100</v>
+      </c>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35">
+        <v>1</v>
+      </c>
+      <c r="L26" s="35">
+        <v>190</v>
+      </c>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="20">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="20">
+        <v>150</v>
+      </c>
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20">
+        <v>1</v>
+      </c>
+      <c r="U26" s="20">
+        <v>240</v>
+      </c>
+      <c r="V26" s="20"/>
+      <c r="W26" s="20"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="20">
+        <v>100</v>
+      </c>
+      <c r="AA26" s="20"/>
+      <c r="AB26" s="20"/>
+      <c r="AC26" s="20">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="20">
+        <v>190</v>
+      </c>
+      <c r="AE26" s="35"/>
+      <c r="AF26" s="35"/>
+      <c r="AG26" s="35"/>
+      <c r="AH26" s="35"/>
+      <c r="AI26" s="35"/>
+      <c r="AJ26" s="35"/>
+      <c r="AK26" s="35"/>
+      <c r="AL26" s="35"/>
+      <c r="AM26" s="35"/>
+    </row>
+    <row r="29" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="L18" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="M18" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="N18" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="O18" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="P18" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q18" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="R18" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="S18" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="T18" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="U18" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="V18" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="W18" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="X18" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y18" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z18" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="AA18" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB18" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="AC18" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="AD18" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE18" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF18" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="AG18" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="AH18" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="AI18" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="AJ18" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="AK18" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="AL18" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="AM18" s="17" t="s">
+      <c r="B30" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="I30" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="J30" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="K30" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="L30" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="M30" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="N30" s="22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="20">
+        <v>200</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A35" s="19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A36" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="G36" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="H36" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="I36" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="J36" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="K36" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="L36" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="M36" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="N36" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="O36" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="P36" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q36" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="R36" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="S36" s="22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A37" s="35" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19">
-        <v>1</v>
-      </c>
-      <c r="H19" s="19">
-        <v>100</v>
-      </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19">
-        <v>1</v>
-      </c>
-      <c r="L19" s="19">
-        <v>190</v>
-      </c>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="20">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="20">
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35">
+        <v>-500</v>
+      </c>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="35"/>
+      <c r="S37" s="35"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" s="35"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35">
+        <v>300</v>
+      </c>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="35"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+      <c r="R38" s="35"/>
+      <c r="S38" s="35"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A39" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35">
+        <v>380</v>
+      </c>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+      <c r="P39" s="35"/>
+      <c r="Q39" s="35"/>
+      <c r="R39" s="35"/>
+      <c r="S39" s="35"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A40" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35">
+        <v>500</v>
+      </c>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="35"/>
+      <c r="S40" s="35"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A41" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23">
+        <v>500</v>
+      </c>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
+      <c r="P41" s="23"/>
+      <c r="Q41" s="23"/>
+      <c r="R41" s="23"/>
+      <c r="S41" s="23"/>
+    </row>
+    <row r="43" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="H44" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="I44" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="J44" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="K44" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="L44" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="M44" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="N44" s="22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B45" s="20">
+        <v>550</v>
+      </c>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="20"/>
+    </row>
+    <row r="47" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20">
-        <v>1</v>
-      </c>
-      <c r="U19" s="20">
-        <v>240</v>
-      </c>
-      <c r="V19" s="20"/>
-      <c r="W19" s="20"/>
-      <c r="X19" s="20"/>
-      <c r="Y19" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z19" s="20">
-        <v>100</v>
-      </c>
-      <c r="AA19" s="20"/>
-      <c r="AB19" s="20"/>
-      <c r="AC19" s="20">
-        <v>1</v>
-      </c>
-      <c r="AD19" s="20">
-        <v>190</v>
-      </c>
-      <c r="AE19" s="19"/>
-      <c r="AF19" s="19"/>
-      <c r="AG19" s="19"/>
-      <c r="AH19" s="19"/>
-      <c r="AI19" s="19"/>
-      <c r="AJ19" s="19"/>
-      <c r="AK19" s="19"/>
-      <c r="AL19" s="19"/>
-      <c r="AM19" s="19"/>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="D48" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F48" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="H48" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="I48" s="37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" s="35">
+        <v>500</v>
+      </c>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" s="35">
+        <v>600</v>
+      </c>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" s="26"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" s="26"/>
+    </row>
+    <row r="53" spans="1:14" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="G54" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="H54" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="I54" s="22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="27"/>
+      <c r="I58" s="27"/>
+      <c r="J58" s="27"/>
+      <c r="K58" s="27"/>
+      <c r="L58" s="27"/>
+      <c r="M58" s="27"/>
+      <c r="N58" s="27"/>
+    </row>
+    <row r="59" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D59" s="22" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="24" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="22" t="s">
+      <c r="E59" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="F59" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="G59" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="H59" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="I59" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="J59" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="E25" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="H25" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="I25" s="22" t="s">
+      <c r="K59" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="J25" s="22" t="s">
+      <c r="L59" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="K25" s="22" t="s">
+      <c r="M59" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="N59" s="22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" s="20">
+        <v>700</v>
+      </c>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="K60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="20"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A61" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="23">
+        <v>700</v>
+      </c>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="L25" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="M25" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="N25" s="22" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="20">
-        <v>200</v>
-      </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-    </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-    </row>
-    <row r="34" spans="1:14" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="G35" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="H35" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="I35" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="J35" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="K35" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="L35" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="M35" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="N35" s="22" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F39" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="H39" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="I39" s="22" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="26"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="26"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" s="26"/>
-    </row>
-    <row r="44" spans="1:14" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="E45" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F45" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="G45" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="H45" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="I45" s="22" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A49" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
-      <c r="L49" s="30"/>
-      <c r="M49" s="30"/>
-      <c r="N49" s="30"/>
-    </row>
-    <row r="50" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B50" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="F50" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="G50" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="H50" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="I50" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="J50" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="K50" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="L50" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="M50" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="N50" s="22" t="s">
-        <v>141</v>
-      </c>
+      <c r="K61" s="23"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="23"/>
+      <c r="N61" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
included shell tables of impact of ablation on the cohort and of building blocks on flares (currently Tables 8 and 9)
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_components_flare_TD_E_GRAVES_AESI.xlsx
+++ b/i_codebooks/D3_components_flare_TD_E_GRAVES_AESI.xlsx
@@ -152,9 +152,6 @@
     <t>most recent date when a diagnostic code of flare has been recorded</t>
   </si>
   <si>
-    <t>start_DP_ANTITHYROID</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>last_TP_RADIOIODINEABLA_AESI</t>
   </si>
   <si>
-    <t>most recent date when a diagnostic code of TP_THYROIDECTOMY_AESII has been recorded</t>
-  </si>
-  <si>
     <t>most recent date of a record of TP_RADIOIODINEABLA_AESI</t>
   </si>
   <si>
@@ -630,6 +624,12 @@
   </si>
   <si>
     <t>P03</t>
+  </si>
+  <si>
+    <t>last_DP_ANTITHYROID</t>
+  </si>
+  <si>
+    <t>most recent date when a diagnostic code of TP_THYROIDECTOMY_AESI has been recorded</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1162,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -1170,7 +1170,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1178,7 +1178,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1186,7 +1186,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1194,7 +1194,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1237,10 +1237,10 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1305,7 +1305,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>34</v>
@@ -1316,7 +1316,7 @@
         <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1349,324 +1349,324 @@
         <v>40</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>41</v>
+        <v>199</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="C10" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>52</v>
+        <v>200</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>53</v>
-      </c>
       <c r="C12" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>166</v>
-      </c>
       <c r="C21" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>167</v>
-      </c>
       <c r="C22" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>177</v>
-      </c>
       <c r="C23" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1713,10 +1713,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1725,77 +1725,77 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
         <v>90</v>
       </c>
-      <c r="B6" t="s">
-        <v>92</v>
-      </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -1829,8 +1829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AM61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1864,7 +1864,7 @@
         <v>38</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>31</v>
@@ -1879,81 +1879,81 @@
         <v>39</v>
       </c>
       <c r="H2" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="J2" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>46</v>
-      </c>
       <c r="K2" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="29" t="s">
-        <v>51</v>
-      </c>
       <c r="M2" s="30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N2" s="30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O2" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="R2" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="Q2" s="31" t="s">
+      <c r="S2" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="R2" s="31" t="s">
+      <c r="T2" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="S2" s="31" t="s">
+      <c r="U2" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="V2" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="W2" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="X2" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="U2" s="31" t="s">
+      <c r="Y2" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB2" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC2" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="V2" s="29" t="s">
+      <c r="AD2" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="W2" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="X2" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y2" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z2" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA2" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB2" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC2" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="AD2" s="31" t="s">
+      <c r="AE2" s="32" t="s">
         <v>173</v>
-      </c>
-      <c r="AE2" s="32" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" s="33">
         <v>100</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" s="33">
         <v>100</v>
@@ -2053,7 +2053,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B5" s="32">
         <v>200</v>
@@ -2100,7 +2100,7 @@
     </row>
     <row r="6" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B6" s="32">
         <v>200</v>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="G6" s="32"/>
       <c r="H6" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="32">
         <v>300</v>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="7" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B7" s="32">
         <v>200</v>
@@ -2202,7 +2202,7 @@
     </row>
     <row r="8" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B8" s="32">
         <v>200</v>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="9" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" s="32">
         <v>200</v>
@@ -2272,7 +2272,7 @@
       </c>
       <c r="G9" s="32"/>
       <c r="H9" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="32">
         <v>500</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B10" s="32">
         <v>200</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B11" s="32">
         <v>200</v>
@@ -2406,7 +2406,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B12" s="32">
         <v>200</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="13" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B13" s="33">
         <v>100</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="14" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B14" s="33">
         <v>100</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="15" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B15" s="33">
         <v>100</v>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="16" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B16" s="33">
         <v>100</v>
@@ -2661,7 +2661,7 @@
     </row>
     <row r="17" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B17" s="33">
         <v>100</v>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="18" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B18" s="33">
         <v>100</v>
@@ -2769,7 +2769,7 @@
     </row>
     <row r="22" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:39" ht="158.4" x14ac:dyDescent="0.3">
@@ -2777,123 +2777,123 @@
         <v>28</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D23" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="G23" s="17" t="s">
         <v>101</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>103</v>
       </c>
       <c r="H23" s="17" t="s">
         <v>38</v>
       </c>
       <c r="I23" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="K23" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="J23" s="17" t="s">
+      <c r="L23" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="K23" s="17" t="s">
+      <c r="M23" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="L23" s="17" t="s">
+      <c r="N23" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="M23" s="17" t="s">
+      <c r="O23" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="N23" s="17" t="s">
+      <c r="P23" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="O23" s="17" t="s">
+      <c r="Q23" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="P23" s="17" t="s">
+      <c r="R23" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="Q23" s="17" t="s">
+      <c r="S23" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="R23" s="17" t="s">
+      <c r="T23" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="S23" s="17" t="s">
+      <c r="U23" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="T23" s="17" t="s">
+      <c r="V23" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="U23" s="17" t="s">
+      <c r="W23" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="V23" s="17" t="s">
+      <c r="X23" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="W23" s="17" t="s">
+      <c r="Y23" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="X23" s="17" t="s">
+      <c r="Z23" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="Y23" s="17" t="s">
+      <c r="AA23" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="Z23" s="17" t="s">
+      <c r="AB23" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="AA23" s="17" t="s">
+      <c r="AC23" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="AB23" s="17" t="s">
+      <c r="AD23" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="AC23" s="17" t="s">
+      <c r="AE23" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="AD23" s="17" t="s">
+      <c r="AF23" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="AE23" s="17" t="s">
+      <c r="AG23" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="AF23" s="17" t="s">
+      <c r="AH23" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="AG23" s="17" t="s">
+      <c r="AI23" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="AH23" s="17" t="s">
+      <c r="AJ23" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="AI23" s="17" t="s">
+      <c r="AK23" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="AJ23" s="17" t="s">
+      <c r="AL23" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="AK23" s="17" t="s">
+      <c r="AM23" s="17" t="s">
         <v>132</v>
-      </c>
-      <c r="AL23" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="AM23" s="17" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" s="35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24" s="35"/>
       <c r="C24" s="35">
@@ -2962,7 +2962,7 @@
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="23">
@@ -3015,7 +3015,7 @@
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" s="35" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B26" s="35"/>
       <c r="C26" s="35">
@@ -3084,7 +3084,7 @@
     </row>
     <row r="29" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
@@ -3092,48 +3092,48 @@
         <v>28</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="F30" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="G30" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I30" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="J30" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="K30" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="L30" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="E30" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="H30" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="I30" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="J30" s="22" t="s">
+      <c r="M30" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="K30" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="L30" s="22" t="s">
+      <c r="N30" s="22" t="s">
         <v>138</v>
-      </c>
-      <c r="M30" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="N30" s="22" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B31" s="20">
         <v>200</v>
@@ -3146,7 +3146,7 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
       <c r="J31" s="20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
@@ -3155,7 +3155,7 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
@@ -3163,63 +3163,63 @@
         <v>28</v>
       </c>
       <c r="B36" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="F36" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="D36" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="23" t="s">
+      <c r="G36" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="F36" s="23" t="s">
+      <c r="H36" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="G36" s="23" t="s">
+      <c r="I36" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="H36" s="23" t="s">
+      <c r="J36" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="I36" s="23" t="s">
+      <c r="K36" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="J36" s="23" t="s">
+      <c r="L36" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="K36" s="23" t="s">
+      <c r="M36" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="N36" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="L36" s="23" t="s">
+      <c r="O36" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="M36" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="N36" s="23" t="s">
+      <c r="P36" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="O36" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="P36" s="23" t="s">
-        <v>194</v>
-      </c>
       <c r="Q36" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="R36" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="S36" s="22" t="s">
         <v>138</v>
-      </c>
-      <c r="R36" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="S36" s="22" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B37" s="35"/>
       <c r="C37" s="35"/>
@@ -3244,7 +3244,7 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B38" s="35"/>
       <c r="C38" s="35"/>
@@ -3269,7 +3269,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B39" s="35"/>
       <c r="C39" s="35"/>
@@ -3294,7 +3294,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B40" s="35"/>
       <c r="C40" s="35"/>
@@ -3319,7 +3319,7 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="23"/>
@@ -3344,7 +3344,7 @@
     </row>
     <row r="43" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
@@ -3352,48 +3352,48 @@
         <v>28</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C44" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="G44" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="H44" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I44" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="J44" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="K44" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="L44" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="E44" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="F44" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="G44" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="H44" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="I44" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="J44" s="22" t="s">
+      <c r="M44" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="K44" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="L44" s="22" t="s">
+      <c r="N44" s="22" t="s">
         <v>138</v>
-      </c>
-      <c r="M44" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="N44" s="22" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B45" s="20">
         <v>550</v>
@@ -3406,7 +3406,7 @@
       <c r="H45" s="20"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K45" s="20"/>
       <c r="L45" s="20"/>
@@ -3415,7 +3415,7 @@
     </row>
     <row r="47" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A47" s="24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.3">
@@ -3423,33 +3423,33 @@
         <v>28</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C48" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="G48" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="D48" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="E48" s="21" t="s">
+      <c r="H48" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="I48" s="37" t="s">
         <v>138</v>
-      </c>
-      <c r="F48" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="G48" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="H48" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="I48" s="37" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B49" s="35">
         <v>500</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B50" s="35">
         <v>600</v>
@@ -3485,7 +3485,7 @@
     </row>
     <row r="53" spans="1:14" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
@@ -3493,33 +3493,33 @@
         <v>28</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C54" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="G54" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="D54" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="E54" s="21" t="s">
+      <c r="H54" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="I54" s="22" t="s">
         <v>138</v>
-      </c>
-      <c r="F54" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="G54" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="H54" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="I54" s="22" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B58" s="27"/>
       <c r="C58" s="27"/>
@@ -3540,48 +3540,48 @@
         <v>28</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C59" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="F59" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="G59" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="H59" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I59" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="J59" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="K59" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="L59" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="E59" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="F59" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="G59" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="H59" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="I59" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="J59" s="22" t="s">
+      <c r="M59" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="K59" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="L59" s="22" t="s">
+      <c r="N59" s="22" t="s">
         <v>138</v>
-      </c>
-      <c r="M59" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="N59" s="22" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B60" s="20">
         <v>700</v>
@@ -3594,7 +3594,7 @@
       <c r="H60" s="20"/>
       <c r="I60" s="20"/>
       <c r="J60" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K60" s="20"/>
       <c r="L60" s="20"/>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B61" s="23">
         <v>700</v>
@@ -3616,7 +3616,7 @@
       <c r="H61" s="23"/>
       <c r="I61" s="23"/>
       <c r="J61" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K61" s="23"/>
       <c r="L61" s="23"/>

</xml_diff>